<commit_message>
Ran Region Results Again
</commit_message>
<xml_diff>
--- a/Figures/Region_Results/Relevant_var_CovIndex_Region.xlsx
+++ b/Figures/Region_Results/Relevant_var_CovIndex_Region.xlsx
@@ -42,157 +42,157 @@
     <t xml:space="preserve">Lasso</t>
   </si>
   <si>
+    <t xml:space="preserve">Continent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO_COV_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO_COV_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO_COV_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Cone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Latin Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOC13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COV6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andean Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECON2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost_gam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XGBoost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latin Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
     <t xml:space="preserve">Americas</t>
   </si>
   <si>
-    <t xml:space="preserve">ECON7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHO_COV_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHO_COV_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECON1</t>
-  </si>
-  <si>
     <t xml:space="preserve">WHO_COV_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECON8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Cone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non Latin Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEALTH15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOC13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECON6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COV6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECON5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECON4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andean Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECON2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boost_gam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XGBoost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latin Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Continent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHO_COV_4</t>
   </si>
   <si>
     <t xml:space="preserve">metrics</t>
@@ -582,7 +582,7 @@
         <v>49</v>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -594,7 +594,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.553264341118228</v>
+        <v>-0.456584204714751</v>
       </c>
     </row>
     <row r="3">
@@ -605,7 +605,7 @@
         <v>49</v>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -617,7 +617,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.132825850993044</v>
+        <v>-0.0987335170927507</v>
       </c>
     </row>
     <row r="4">
@@ -628,7 +628,7 @@
         <v>49</v>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -640,7 +640,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G4" t="n">
-        <v>-310.276164619221</v>
+        <v>-351.025439780704</v>
       </c>
     </row>
     <row r="5">
@@ -651,7 +651,7 @@
         <v>49</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -663,7 +663,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G5" t="n">
-        <v>-7.36153298982804</v>
+        <v>1.08304995602966</v>
       </c>
     </row>
     <row r="6">
@@ -674,7 +674,7 @@
         <v>49</v>
       </c>
       <c r="C6" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -686,7 +686,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G6" t="n">
-        <v>1.32895567718543</v>
+        <v>0.000371367037972821</v>
       </c>
     </row>
     <row r="7">
@@ -697,7 +697,7 @@
         <v>49</v>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -709,7 +709,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00390502280518578</v>
+        <v>0.783581169157851</v>
       </c>
     </row>
     <row r="8">
@@ -720,7 +720,7 @@
         <v>49</v>
       </c>
       <c r="C8" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -732,7 +732,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G8" t="n">
-        <v>0.622802510478115</v>
+        <v>-0.0000947226671947312</v>
       </c>
     </row>
     <row r="9">
@@ -743,7 +743,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -755,7 +755,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0111662729491523</v>
+        <v>-0.0000821322857415857</v>
       </c>
     </row>
     <row r="10">
@@ -766,7 +766,7 @@
         <v>49</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -778,7 +778,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.000239436210981199</v>
+        <v>10.1338816118844</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>49</v>
       </c>
       <c r="C11" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -801,7 +801,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G11" t="n">
-        <v>10.0320733499019</v>
+        <v>-0.00124972659167292</v>
       </c>
     </row>
     <row r="12">
@@ -812,7 +812,7 @@
         <v>49</v>
       </c>
       <c r="C12" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -824,7 +824,7 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.266416597676502</v>
+        <v>-0.387980330012543</v>
       </c>
     </row>
     <row r="13">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -847,30 +847,30 @@
         <v>0.432876128108306</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.256594061047733</v>
+        <v>-0.709146272241574</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="n">
+        <v>36</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="n">
-        <v>49</v>
-      </c>
-      <c r="C14" t="n">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
       <c r="F14" t="n">
-        <v>0.432876128108306</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G14" t="n">
-        <v>5.95270917942259</v>
+        <v>-0.634539731778912</v>
       </c>
     </row>
     <row r="15">
@@ -878,22 +878,22 @@
         <v>22</v>
       </c>
       <c r="B15" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C15" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F15" t="n">
-        <v>0.432876128108306</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.32548716420511</v>
+        <v>37.5955406472182</v>
       </c>
     </row>
     <row r="16">
@@ -901,206 +901,206 @@
         <v>23</v>
       </c>
       <c r="B16" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.33544337176238</v>
+        <v>0.0296294757436788</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G17" t="n">
-        <v>3.68302845733606</v>
+        <v>0.0241773941767681</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B18" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.12511741242435</v>
+        <v>-0.267201745096526</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G19" t="n">
-        <v>0.300010776589025</v>
+        <v>-0.725787607694912</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0294758533153931</v>
+        <v>0.00296052294839221</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="n">
+        <v>36</v>
+      </c>
+      <c r="C21" t="n">
         <v>10</v>
       </c>
-      <c r="B21" t="n">
-        <v>33</v>
-      </c>
-      <c r="C21" t="n">
-        <v>32</v>
-      </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>-1.28840644027473</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C22" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G22" t="n">
-        <v>1.01309085736107</v>
+        <v>3.78977009037494</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C23" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0.00657933224657568</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.00135048687149453</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="n">
+        <v>39</v>
+      </c>
+      <c r="C24" t="n">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="n">
-        <v>33</v>
-      </c>
-      <c r="C24" t="n">
-        <v>32</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
       <c r="F24" t="n">
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>-1.33544337176238</v>
       </c>
     </row>
     <row r="25">
@@ -1108,96 +1108,96 @@
         <v>31</v>
       </c>
       <c r="B25" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C25" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>3.68302845733606</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B26" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C26" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>-0.12511741242435</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C27" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>183.388758267875</v>
+        <v>0.300010776589025</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C28" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.0294758533153931</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" t="n">
         <v>33</v>
@@ -1209,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F29" t="n">
         <v>1</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B30" t="n">
         <v>33</v>
@@ -1232,18 +1232,18 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F30" t="n">
         <v>1</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>1.01309085736107</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B31" t="n">
         <v>33</v>
@@ -1255,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F31" t="n">
         <v>1</v>
@@ -1278,7 +1278,7 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F32" t="n">
         <v>1</v>
@@ -1301,7 +1301,7 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F33" t="n">
         <v>1</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B34" t="n">
         <v>33</v>
@@ -1324,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B35" t="n">
         <v>33</v>
@@ -1347,18 +1347,18 @@
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>183.388758267875</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" t="n">
         <v>33</v>
@@ -1370,7 +1370,7 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" t="n">
         <v>33</v>
@@ -1393,7 +1393,7 @@
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B38" t="n">
         <v>33</v>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F38" t="n">
         <v>1</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" t="n">
         <v>33</v>
@@ -1439,7 +1439,7 @@
         <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F39" t="n">
         <v>1</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="n">
         <v>33</v>
@@ -1462,7 +1462,7 @@
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F40" t="n">
         <v>1</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B41" t="n">
         <v>33</v>
@@ -1485,7 +1485,7 @@
         <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B42" t="n">
         <v>33</v>
@@ -1508,7 +1508,7 @@
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B43" t="n">
         <v>33</v>
@@ -1531,7 +1531,7 @@
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B44" t="n">
         <v>33</v>
@@ -1554,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B45" t="n">
         <v>33</v>
@@ -1577,7 +1577,7 @@
         <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B46" t="n">
         <v>33</v>
@@ -1600,7 +1600,7 @@
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F46" t="n">
         <v>1</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>33</v>
@@ -1623,7 +1623,7 @@
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F47" t="n">
         <v>1</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B48" t="n">
         <v>33</v>
@@ -1646,7 +1646,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B49" t="n">
         <v>33</v>
@@ -1669,7 +1669,7 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F49" t="n">
         <v>1</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="B50" t="n">
         <v>33</v>
@@ -1692,7 +1692,7 @@
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -1715,7 +1715,7 @@
         <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F51" t="n">
         <v>1</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B52" t="n">
         <v>33</v>
@@ -1738,7 +1738,7 @@
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F52" t="n">
         <v>1</v>
@@ -1749,197 +1749,197 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B53" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C53" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F53" t="n">
         <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>0.220388545101995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B54" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C54" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s">
         <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F54" t="n">
         <v>1</v>
       </c>
       <c r="G54" t="n">
-        <v>1.2873971792188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B55" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C55" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D55" t="s">
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F55" t="n">
         <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>-0.171032675256604</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B56" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C56" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
       </c>
       <c r="G56" t="n">
-        <v>1.33356955234299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B57" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C57" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
       </c>
       <c r="G57" t="n">
-        <v>-1.84338174991008</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B58" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C58" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
         <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F58" t="n">
         <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>0.000153310576629999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B59" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C59" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F59" t="n">
         <v>1</v>
       </c>
       <c r="G59" t="n">
-        <v>-0.687327631966658</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B60" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C60" t="n">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s">
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G60" t="n">
-        <v>-0.131389435015302</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B61" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C61" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D61" t="s">
         <v>8</v>
@@ -1948,21 +1948,21 @@
         <v>49</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G61" t="n">
-        <v>2.66708674571704</v>
+        <v>0.220388545101995</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B62" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C62" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D62" t="s">
         <v>8</v>
@@ -1971,21 +1971,21 @@
         <v>49</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G62" t="n">
-        <v>-0.277895069993041</v>
+        <v>1.2873971792188</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B63" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C63" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
         <v>8</v>
@@ -1994,21 +1994,21 @@
         <v>49</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
-        <v>0.040992411581161</v>
+        <v>-0.171032675256604</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B64" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C64" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
         <v>8</v>
@@ -2017,21 +2017,21 @@
         <v>49</v>
       </c>
       <c r="F64" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G64" t="n">
-        <v>-125.537767974376</v>
+        <v>1.33356955234299</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C65" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
         <v>8</v>
@@ -2040,21 +2040,21 @@
         <v>49</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G65" t="n">
-        <v>161.775374129486</v>
+        <v>-1.84338174991008</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B66" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C66" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
@@ -2063,21 +2063,21 @@
         <v>49</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G66" t="n">
-        <v>-0.362357265778621</v>
+        <v>0.000153310576629999</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B67" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
@@ -2086,15 +2086,15 @@
         <v>49</v>
       </c>
       <c r="F67" t="n">
-        <v>0.0001</v>
+        <v>1</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.425257082005654</v>
+        <v>-0.687327631966658</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B68" t="n">
         <v>40</v>
@@ -2106,294 +2106,294 @@
         <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F68" t="n">
         <v>0.0001</v>
       </c>
       <c r="G68" t="n">
-        <v>-0.00225285416664765</v>
+        <v>-0.131389435015302</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B69" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C69" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
         <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F69" t="n">
-        <v>0.432876128108306</v>
+        <v>0.0001</v>
       </c>
       <c r="G69" t="n">
-        <v>-0.129977814542115</v>
+        <v>2.66708674571704</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B70" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C70" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F70" t="n">
-        <v>0.432876128108306</v>
+        <v>0.0001</v>
       </c>
       <c r="G70" t="n">
-        <v>-1779.91459129621</v>
+        <v>-0.277895069993041</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B71" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C71" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D71" t="s">
         <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F71" t="n">
-        <v>0.432876128108306</v>
+        <v>0.0001</v>
       </c>
       <c r="G71" t="n">
-        <v>1.29570634709611</v>
+        <v>0.040992411581161</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B72" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C72" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
       </c>
       <c r="E72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F72" t="n">
-        <v>0.432876128108306</v>
+        <v>0.0001</v>
       </c>
       <c r="G72" t="n">
-        <v>34.3208092268016</v>
+        <v>-125.537767974376</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B73" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C73" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E73" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>0.0001</v>
       </c>
       <c r="G73" t="n">
-        <v>13.7114187048752</v>
+        <v>161.775374129486</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B74" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C74" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>0.0001</v>
       </c>
       <c r="G74" t="n">
-        <v>13.6557010107645</v>
+        <v>-0.362357265778621</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B75" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C75" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>0.0001</v>
       </c>
       <c r="G75" t="n">
-        <v>13.0709344401247</v>
+        <v>-0.425257082005654</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B76" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C76" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F76" t="n">
-        <v>1</v>
+        <v>0.0001</v>
       </c>
       <c r="G76" t="n">
-        <v>13.045354358039</v>
+        <v>-0.00225285416664765</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B77" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C77" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
         <v>52</v>
       </c>
-      <c r="E77" t="s">
-        <v>53</v>
-      </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G77" t="n">
-        <v>12.808453861078</v>
+        <v>-0.129977814542115</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B78" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C78" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s">
         <v>52</v>
       </c>
-      <c r="E78" t="s">
-        <v>53</v>
-      </c>
       <c r="F78" t="n">
-        <v>1</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G78" t="n">
-        <v>12.7978273271021</v>
+        <v>-1779.91459129621</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B79" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C79" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" t="s">
         <v>52</v>
       </c>
-      <c r="E79" t="s">
-        <v>53</v>
-      </c>
       <c r="F79" t="n">
-        <v>1</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G79" t="n">
-        <v>11.8392997062197</v>
+        <v>1.29570634709611</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B80" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C80" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" t="s">
         <v>52</v>
       </c>
-      <c r="E80" t="s">
-        <v>53</v>
-      </c>
       <c r="F80" t="n">
-        <v>1</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G80" t="n">
-        <v>11.6441018719214</v>
+        <v>34.3208092268016</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B81" t="n">
         <v>38</v>
@@ -2402,21 +2402,21 @@
         <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E81" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F81" t="n">
         <v>1</v>
       </c>
       <c r="G81" t="n">
-        <v>11.4612108741256</v>
+        <v>13.7114187048752</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B82" t="n">
         <v>38</v>
@@ -2425,21 +2425,21 @@
         <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E82" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
       </c>
       <c r="G82" t="n">
-        <v>10.219083845654</v>
+        <v>13.6557010107645</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B83" t="n">
         <v>38</v>
@@ -2448,21 +2448,21 @@
         <v>18</v>
       </c>
       <c r="D83" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E83" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
       </c>
       <c r="G83" t="n">
-        <v>6.98806865589874</v>
+        <v>13.0709344401247</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B84" t="n">
         <v>38</v>
@@ -2471,21 +2471,21 @@
         <v>18</v>
       </c>
       <c r="D84" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E84" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
       </c>
       <c r="G84" t="n">
-        <v>5.93285427175797</v>
+        <v>13.045354358039</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B85" t="n">
         <v>38</v>
@@ -2494,21 +2494,21 @@
         <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E85" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F85" t="n">
         <v>1</v>
       </c>
       <c r="G85" t="n">
-        <v>5.45813645493968</v>
+        <v>12.808453861078</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B86" t="n">
         <v>38</v>
@@ -2517,21 +2517,21 @@
         <v>18</v>
       </c>
       <c r="D86" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E86" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F86" t="n">
         <v>1</v>
       </c>
       <c r="G86" t="n">
-        <v>5.04833216400577</v>
+        <v>12.7978273271021</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B87" t="n">
         <v>38</v>
@@ -2540,21 +2540,21 @@
         <v>18</v>
       </c>
       <c r="D87" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F87" t="n">
         <v>1</v>
       </c>
       <c r="G87" t="n">
-        <v>4.73327569968996</v>
+        <v>11.8392997062197</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B88" t="n">
         <v>38</v>
@@ -2563,21 +2563,21 @@
         <v>18</v>
       </c>
       <c r="D88" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E88" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F88" t="n">
         <v>1</v>
       </c>
       <c r="G88" t="n">
-        <v>3.13635711445594</v>
+        <v>11.6441018719214</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B89" t="n">
         <v>38</v>
@@ -2586,21 +2586,21 @@
         <v>18</v>
       </c>
       <c r="D89" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E89" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
       </c>
       <c r="G89" t="n">
-        <v>3.13635711445594</v>
+        <v>11.4612108741256</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B90" t="n">
         <v>38</v>
@@ -2609,214 +2609,214 @@
         <v>18</v>
       </c>
       <c r="D90" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E90" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>2.93592924370171</v>
+        <v>10.219083845654</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B91" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C91" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D91" t="s">
+        <v>53</v>
+      </c>
+      <c r="E91" t="s">
         <v>54</v>
       </c>
-      <c r="E91" t="s">
-        <v>55</v>
-      </c>
       <c r="F91" t="n">
         <v>1</v>
       </c>
       <c r="G91" t="n">
-        <v>0.444225881748798</v>
+        <v>6.98806865589874</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B92" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C92" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D92" t="s">
+        <v>53</v>
+      </c>
+      <c r="E92" t="s">
         <v>54</v>
       </c>
-      <c r="E92" t="s">
-        <v>55</v>
-      </c>
       <c r="F92" t="n">
         <v>1</v>
       </c>
       <c r="G92" t="n">
-        <v>0.290274062764366</v>
+        <v>5.93285427175797</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B93" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C93" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D93" t="s">
+        <v>53</v>
+      </c>
+      <c r="E93" t="s">
         <v>54</v>
       </c>
-      <c r="E93" t="s">
-        <v>55</v>
-      </c>
       <c r="F93" t="n">
         <v>1</v>
       </c>
       <c r="G93" t="n">
-        <v>0.226174065569105</v>
+        <v>5.45813645493968</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B94" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C94" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D94" t="s">
+        <v>53</v>
+      </c>
+      <c r="E94" t="s">
         <v>54</v>
       </c>
-      <c r="E94" t="s">
-        <v>55</v>
-      </c>
       <c r="F94" t="n">
         <v>1</v>
       </c>
       <c r="G94" t="n">
-        <v>0.0337140027389249</v>
+        <v>5.04833216400577</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B95" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C95" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D95" t="s">
+        <v>53</v>
+      </c>
+      <c r="E95" t="s">
         <v>54</v>
       </c>
-      <c r="E95" t="s">
-        <v>55</v>
-      </c>
       <c r="F95" t="n">
         <v>1</v>
       </c>
       <c r="G95" t="n">
-        <v>0.00249936769452927</v>
+        <v>4.73327569968996</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B96" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C96" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D96" t="s">
+        <v>53</v>
+      </c>
+      <c r="E96" t="s">
         <v>54</v>
       </c>
-      <c r="E96" t="s">
-        <v>55</v>
-      </c>
       <c r="F96" t="n">
         <v>1</v>
       </c>
       <c r="G96" t="n">
-        <v>0.00211733955789904</v>
+        <v>3.13635711445594</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B97" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C97" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D97" t="s">
+        <v>53</v>
+      </c>
+      <c r="E97" t="s">
         <v>54</v>
       </c>
-      <c r="E97" t="s">
-        <v>56</v>
-      </c>
       <c r="F97" t="n">
         <v>1</v>
       </c>
       <c r="G97" t="n">
-        <v>0.996228033920579</v>
+        <v>3.13635711445594</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>46</v>
+      </c>
+      <c r="B98" t="n">
         <v>38</v>
       </c>
-      <c r="B98" t="n">
-        <v>39</v>
-      </c>
       <c r="C98" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D98" t="s">
+        <v>53</v>
+      </c>
+      <c r="E98" t="s">
         <v>54</v>
       </c>
-      <c r="E98" t="s">
-        <v>56</v>
-      </c>
       <c r="F98" t="n">
         <v>1</v>
       </c>
       <c r="G98" t="n">
-        <v>0.00217340410668898</v>
+        <v>2.93592924370171</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B99" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C99" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D99" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E99" t="s">
         <v>56</v>
@@ -2825,294 +2825,294 @@
         <v>1</v>
       </c>
       <c r="G99" t="n">
-        <v>0.000899143536448235</v>
+        <v>0.444225881748798</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B100" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C100" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E100" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F100" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G100" t="n">
-        <v>-0.456584204714751</v>
+        <v>0.290274062764366</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B101" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C101" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D101" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E101" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F101" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G101" t="n">
-        <v>-0.0987335170927507</v>
+        <v>0.226174065569105</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B102" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C102" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D102" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E102" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F102" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G102" t="n">
-        <v>-351.025439780704</v>
+        <v>0.0337140027389249</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B103" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C103" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D103" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E103" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F103" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G103" t="n">
-        <v>1.08304995602966</v>
+        <v>0.00249936769452927</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B104" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C104" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D104" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E104" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F104" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G104" t="n">
-        <v>0.000371367037972821</v>
+        <v>0.00211733955789904</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B105" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C105" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E105" t="s">
         <v>57</v>
       </c>
       <c r="F105" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G105" t="n">
-        <v>0.783581169157851</v>
+        <v>0.996228033920579</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B106" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C106" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E106" t="s">
         <v>57</v>
       </c>
       <c r="F106" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G106" t="n">
-        <v>-0.0000947226671947312</v>
+        <v>0.00217340410668898</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B107" t="n">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C107" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="E107" t="s">
         <v>57</v>
       </c>
       <c r="F107" t="n">
-        <v>0.432876128108306</v>
+        <v>1</v>
       </c>
       <c r="G107" t="n">
-        <v>-0.0000821322857415857</v>
+        <v>0.000899143536448235</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B108" t="n">
         <v>49</v>
       </c>
       <c r="C108" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D108" t="s">
         <v>8</v>
       </c>
       <c r="E108" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F108" t="n">
         <v>0.432876128108306</v>
       </c>
       <c r="G108" t="n">
-        <v>10.1338816118844</v>
+        <v>-0.553264341118228</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B109" t="n">
         <v>49</v>
       </c>
       <c r="C109" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D109" t="s">
         <v>8</v>
       </c>
       <c r="E109" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F109" t="n">
         <v>0.432876128108306</v>
       </c>
       <c r="G109" t="n">
-        <v>-0.00124972659167292</v>
+        <v>-0.132825850993044</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B110" t="n">
         <v>49</v>
       </c>
       <c r="C110" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D110" t="s">
         <v>8</v>
       </c>
       <c r="E110" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F110" t="n">
         <v>0.432876128108306</v>
       </c>
       <c r="G110" t="n">
-        <v>-0.387980330012543</v>
+        <v>-310.276164619221</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B111" t="n">
         <v>49</v>
       </c>
       <c r="C111" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D111" t="s">
         <v>8</v>
       </c>
       <c r="E111" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F111" t="n">
         <v>0.432876128108306</v>
       </c>
       <c r="G111" t="n">
-        <v>-0.709146272241574</v>
+        <v>-7.36153298982804</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B112" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C112" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D112" t="s">
         <v>8</v>
@@ -3121,21 +3121,21 @@
         <v>58</v>
       </c>
       <c r="F112" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G112" t="n">
-        <v>-0.634539731778912</v>
+        <v>1.32895567718543</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B113" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C113" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D113" t="s">
         <v>8</v>
@@ -3144,21 +3144,21 @@
         <v>58</v>
       </c>
       <c r="F113" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G113" t="n">
-        <v>37.5955406472182</v>
+        <v>0.00390502280518578</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B114" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C114" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D114" t="s">
         <v>8</v>
@@ -3167,21 +3167,21 @@
         <v>58</v>
       </c>
       <c r="F114" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G114" t="n">
-        <v>0.0296294757436788</v>
+        <v>0.622802510478115</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B115" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C115" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D115" t="s">
         <v>8</v>
@@ -3190,21 +3190,21 @@
         <v>58</v>
       </c>
       <c r="F115" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G115" t="n">
-        <v>0.0241773941767681</v>
+        <v>-0.0111662729491523</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" t="n">
+        <v>49</v>
+      </c>
+      <c r="C116" t="n">
         <v>14</v>
-      </c>
-      <c r="B116" t="n">
-        <v>36</v>
-      </c>
-      <c r="C116" t="n">
-        <v>10</v>
       </c>
       <c r="D116" t="s">
         <v>8</v>
@@ -3213,21 +3213,21 @@
         <v>58</v>
       </c>
       <c r="F116" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G116" t="n">
-        <v>-0.267201745096526</v>
+        <v>-0.000239436210981199</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B117" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C117" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D117" t="s">
         <v>8</v>
@@ -3236,21 +3236,21 @@
         <v>58</v>
       </c>
       <c r="F117" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G117" t="n">
-        <v>-0.725787607694912</v>
+        <v>10.0320733499019</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B118" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C118" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D118" t="s">
         <v>8</v>
@@ -3259,21 +3259,21 @@
         <v>58</v>
       </c>
       <c r="F118" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G118" t="n">
-        <v>0.00296052294839221</v>
+        <v>-0.266416597676502</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B119" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C119" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D119" t="s">
         <v>8</v>
@@ -3282,21 +3282,21 @@
         <v>58</v>
       </c>
       <c r="F119" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G119" t="n">
-        <v>-1.28840644027473</v>
+        <v>-0.256594061047733</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B120" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C120" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D120" t="s">
         <v>8</v>
@@ -3305,21 +3305,21 @@
         <v>58</v>
       </c>
       <c r="F120" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G120" t="n">
-        <v>3.78977009037494</v>
+        <v>5.95270917942259</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B121" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C121" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D121" t="s">
         <v>8</v>
@@ -3328,10 +3328,10 @@
         <v>58</v>
       </c>
       <c r="F121" t="n">
-        <v>0.00657933224657568</v>
+        <v>0.432876128108306</v>
       </c>
       <c r="G121" t="n">
-        <v>0.00135048687149453</v>
+        <v>-1.32548716420511</v>
       </c>
     </row>
   </sheetData>
@@ -3376,19 +3376,19 @@
         <v>67</v>
       </c>
       <c r="B2" t="n">
-        <v>1.4274718624925</v>
+        <v>1.38870719665374</v>
       </c>
       <c r="C2" t="n">
-        <v>0.503838447130369</v>
+        <v>0.508188900576554</v>
       </c>
       <c r="D2" t="n">
-        <v>0.716343499210468</v>
+        <v>0.6964878859709</v>
       </c>
       <c r="E2" t="n">
-        <v>1.15271445462066</v>
+        <v>0.868901052155808</v>
       </c>
       <c r="F2" t="n">
-        <v>1.45602214268836</v>
+        <v>2.25097408075245</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -3399,19 +3399,19 @@
         <v>68</v>
       </c>
       <c r="B3" t="n">
-        <v>1.24900141447276</v>
+        <v>1.2158214357912</v>
       </c>
       <c r="C3" t="n">
-        <v>0.427428638090227</v>
+        <v>0.411387203070234</v>
       </c>
       <c r="D3" t="n">
-        <v>0.684209736113797</v>
+        <v>0.661732421804452</v>
       </c>
       <c r="E3" t="n">
-        <v>0.991241582492815</v>
+        <v>0.74700931160373</v>
       </c>
       <c r="F3" t="n">
-        <v>1.25186859178974</v>
+        <v>2.04921397688923</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -3422,22 +3422,22 @@
         <v>67</v>
       </c>
       <c r="B4" t="n">
-        <v>0.940227655763752</v>
+        <v>1.9059503620883</v>
       </c>
       <c r="C4" t="n">
-        <v>0.617440880612572</v>
+        <v>1.15590032650474</v>
       </c>
       <c r="D4" t="n">
-        <v>0.646733226393177</v>
+        <v>1.19746808526891</v>
       </c>
       <c r="E4" t="n">
-        <v>1.52428314907212</v>
+        <v>4.14450605273849</v>
       </c>
       <c r="F4" t="n">
-        <v>1.47678125951783</v>
+        <v>2.37707039900009</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -3445,22 +3445,22 @@
         <v>68</v>
       </c>
       <c r="B5" t="n">
-        <v>0.709271186874755</v>
+        <v>1.42251699055475</v>
       </c>
       <c r="C5" t="n">
-        <v>0.523142998891412</v>
+        <v>1.07293041085584</v>
       </c>
       <c r="D5" t="n">
-        <v>0.63501337025615</v>
+        <v>1.1862966652738</v>
       </c>
       <c r="E5" t="n">
-        <v>1.37082452455089</v>
+        <v>3.82166462142928</v>
       </c>
       <c r="F5" t="n">
-        <v>1.33565811168123</v>
+        <v>2.05671887868381</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -3468,22 +3468,22 @@
         <v>67</v>
       </c>
       <c r="B6" t="n">
-        <v>2.62586019789187</v>
+        <v>0.940227655763752</v>
       </c>
       <c r="C6" t="n">
-        <v>1.28259572610424</v>
+        <v>0.617440880612572</v>
       </c>
       <c r="D6" t="n">
-        <v>1.36674637708225</v>
+        <v>0.646733226393177</v>
       </c>
       <c r="E6" t="n">
-        <v>2.05383752716801</v>
+        <v>1.52428314907212</v>
       </c>
       <c r="F6" t="n">
-        <v>3.77833472917552</v>
+        <v>1.47678125951783</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
@@ -3491,22 +3491,22 @@
         <v>68</v>
       </c>
       <c r="B7" t="n">
-        <v>2.24604548362101</v>
+        <v>0.709271186874755</v>
       </c>
       <c r="C7" t="n">
-        <v>1.11210490889626</v>
+        <v>0.523142998891412</v>
       </c>
       <c r="D7" t="n">
-        <v>1.3463172708274</v>
+        <v>0.63501337025615</v>
       </c>
       <c r="E7" t="n">
-        <v>1.74069569448126</v>
+        <v>1.37082452455089</v>
       </c>
       <c r="F7" t="n">
-        <v>3.5022074298709</v>
+        <v>1.33565811168123</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -3514,22 +3514,22 @@
         <v>67</v>
       </c>
       <c r="B8" t="n">
-        <v>1.69151953627956</v>
+        <v>2.62586019789187</v>
       </c>
       <c r="C8" t="n">
-        <v>0.847773866390598</v>
+        <v>1.28259572610424</v>
       </c>
       <c r="D8" t="n">
-        <v>1.00301834737396</v>
+        <v>1.36674637708225</v>
       </c>
       <c r="E8" t="n">
-        <v>2.68939135641632</v>
+        <v>2.05383752716801</v>
       </c>
       <c r="F8" t="n">
-        <v>1.26592405640138</v>
+        <v>3.77833472917552</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -3537,22 +3537,22 @@
         <v>68</v>
       </c>
       <c r="B9" t="n">
-        <v>1.36391582914145</v>
+        <v>2.24604548362101</v>
       </c>
       <c r="C9" t="n">
-        <v>0.741176047491368</v>
+        <v>1.11210490889626</v>
       </c>
       <c r="D9" t="n">
-        <v>0.915724189761498</v>
+        <v>1.3463172708274</v>
       </c>
       <c r="E9" t="n">
-        <v>2.43107757251239</v>
+        <v>1.74069569448126</v>
       </c>
       <c r="F9" t="n">
-        <v>0.996393920042902</v>
+        <v>3.5022074298709</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -3560,19 +3560,19 @@
         <v>67</v>
       </c>
       <c r="B10" t="n">
-        <v>2.62922589172816</v>
+        <v>1.69151953627956</v>
       </c>
       <c r="C10" t="n">
-        <v>1.09258073607611</v>
+        <v>0.847773866390598</v>
       </c>
       <c r="D10" t="n">
-        <v>2.11044048104833</v>
+        <v>1.00301834737396</v>
       </c>
       <c r="E10" t="n">
-        <v>1.77143269905613</v>
+        <v>2.68939135641632</v>
       </c>
       <c r="F10" t="n">
-        <v>2.2522312186184</v>
+        <v>1.26592405640138</v>
       </c>
       <c r="G10" t="s">
         <v>49</v>
@@ -3583,19 +3583,19 @@
         <v>68</v>
       </c>
       <c r="B11" t="n">
-        <v>2.26297310280112</v>
+        <v>1.36391582914145</v>
       </c>
       <c r="C11" t="n">
-        <v>0.875359139307768</v>
+        <v>0.741176047491368</v>
       </c>
       <c r="D11" t="n">
-        <v>1.64609787835119</v>
+        <v>0.915724189761498</v>
       </c>
       <c r="E11" t="n">
-        <v>1.47078299513995</v>
+        <v>2.43107757251239</v>
       </c>
       <c r="F11" t="n">
-        <v>1.85987335314342</v>
+        <v>0.996393920042902</v>
       </c>
       <c r="G11" t="s">
         <v>49</v>
@@ -3606,22 +3606,22 @@
         <v>67</v>
       </c>
       <c r="B12" t="n">
-        <v>1.40013924625026</v>
+        <v>2.62922589172816</v>
       </c>
       <c r="C12" t="n">
-        <v>0.82013497422538</v>
+        <v>1.09258073607611</v>
       </c>
       <c r="D12" t="n">
-        <v>0.928152019629306</v>
+        <v>2.11044048104833</v>
       </c>
       <c r="E12" t="n">
-        <v>1.58427282304604</v>
+        <v>1.77143269905613</v>
       </c>
       <c r="F12" t="n">
-        <v>6.77811025377074</v>
+        <v>2.2522312186184</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -3629,22 +3629,22 @@
         <v>68</v>
       </c>
       <c r="B13" t="n">
-        <v>1.24775698187774</v>
+        <v>2.26297310280112</v>
       </c>
       <c r="C13" t="n">
-        <v>0.538001963558091</v>
+        <v>0.875359139307768</v>
       </c>
       <c r="D13" t="n">
-        <v>0.739402829686817</v>
+        <v>1.64609787835119</v>
       </c>
       <c r="E13" t="n">
-        <v>1.41016061990014</v>
+        <v>1.47078299513995</v>
       </c>
       <c r="F13" t="n">
-        <v>6.432714317218</v>
+        <v>1.85987335314342</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
@@ -3652,22 +3652,22 @@
         <v>67</v>
       </c>
       <c r="B14" t="n">
-        <v>0.921238851749306</v>
+        <v>1.40013924625026</v>
       </c>
       <c r="C14" t="n">
-        <v>0.455341626539212</v>
+        <v>0.82013497422538</v>
       </c>
       <c r="D14" t="n">
-        <v>0.667236263403356</v>
+        <v>0.928152019629306</v>
       </c>
       <c r="E14" t="n">
-        <v>0.602229218591013</v>
+        <v>1.58427282304604</v>
       </c>
       <c r="F14" t="n">
-        <v>0.471412814777639</v>
+        <v>6.77811025377074</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
@@ -3675,22 +3675,22 @@
         <v>68</v>
       </c>
       <c r="B15" t="n">
-        <v>0.791404696551979</v>
+        <v>1.24775698187774</v>
       </c>
       <c r="C15" t="n">
-        <v>0.418774612014015</v>
+        <v>0.538001963558091</v>
       </c>
       <c r="D15" t="n">
-        <v>0.520855724321997</v>
+        <v>0.739402829686817</v>
       </c>
       <c r="E15" t="n">
-        <v>0.546054933406747</v>
+        <v>1.41016061990014</v>
       </c>
       <c r="F15" t="n">
-        <v>0.385869792127096</v>
+        <v>6.432714317218</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
@@ -3698,22 +3698,22 @@
         <v>67</v>
       </c>
       <c r="B16" t="n">
-        <v>2.80663167711074</v>
+        <v>0.921238851749306</v>
       </c>
       <c r="C16" t="n">
-        <v>2.40407054595191</v>
+        <v>0.455341626539212</v>
       </c>
       <c r="D16" t="n">
-        <v>1.61393971189421</v>
+        <v>0.667236263403356</v>
       </c>
       <c r="E16" t="n">
-        <v>3.91770996956139</v>
+        <v>0.602229218591013</v>
       </c>
       <c r="F16" t="n">
-        <v>2.58250949299467</v>
+        <v>0.471412814777639</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
@@ -3721,22 +3721,22 @@
         <v>68</v>
       </c>
       <c r="B17" t="n">
-        <v>2.40861471167647</v>
+        <v>0.791404696551979</v>
       </c>
       <c r="C17" t="n">
-        <v>1.9779449035551</v>
+        <v>0.418774612014015</v>
       </c>
       <c r="D17" t="n">
-        <v>1.22294347655203</v>
+        <v>0.520855724321997</v>
       </c>
       <c r="E17" t="n">
-        <v>3.52539505766618</v>
+        <v>0.546054933406747</v>
       </c>
       <c r="F17" t="n">
-        <v>2.20659349786926</v>
+        <v>0.385869792127096</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18">
@@ -3744,19 +3744,19 @@
         <v>67</v>
       </c>
       <c r="B18" t="n">
-        <v>3.28160598481845</v>
+        <v>2.80663167711074</v>
       </c>
       <c r="C18" t="n">
-        <v>0.985474283487416</v>
+        <v>2.40407054595191</v>
       </c>
       <c r="D18" t="n">
-        <v>0.742766328819395</v>
+        <v>1.61393971189421</v>
       </c>
       <c r="E18" t="n">
-        <v>2.77447324631372</v>
+        <v>3.91770996956139</v>
       </c>
       <c r="F18" t="n">
-        <v>4.2940113439009</v>
+        <v>2.58250949299467</v>
       </c>
       <c r="G18" t="s">
         <v>56</v>
@@ -3767,19 +3767,19 @@
         <v>68</v>
       </c>
       <c r="B19" t="n">
-        <v>3.16325549987814</v>
+        <v>2.40861471167647</v>
       </c>
       <c r="C19" t="n">
-        <v>0.891634984267803</v>
+        <v>1.9779449035551</v>
       </c>
       <c r="D19" t="n">
-        <v>0.737215563806988</v>
+        <v>1.22294347655203</v>
       </c>
       <c r="E19" t="n">
-        <v>2.39500190379072</v>
+        <v>3.52539505766618</v>
       </c>
       <c r="F19" t="n">
-        <v>4.13218663561427</v>
+        <v>2.20659349786926</v>
       </c>
       <c r="G19" t="s">
         <v>56</v>
@@ -3790,19 +3790,19 @@
         <v>67</v>
       </c>
       <c r="B20" t="n">
-        <v>1.38870719665374</v>
+        <v>3.28160598481845</v>
       </c>
       <c r="C20" t="n">
-        <v>0.508188900576554</v>
+        <v>0.985474283487416</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6964878859709</v>
+        <v>0.742766328819395</v>
       </c>
       <c r="E20" t="n">
-        <v>0.868901052155808</v>
+        <v>2.77447324631372</v>
       </c>
       <c r="F20" t="n">
-        <v>2.25097408075245</v>
+        <v>4.2940113439009</v>
       </c>
       <c r="G20" t="s">
         <v>57</v>
@@ -3813,19 +3813,19 @@
         <v>68</v>
       </c>
       <c r="B21" t="n">
-        <v>1.2158214357912</v>
+        <v>3.16325549987814</v>
       </c>
       <c r="C21" t="n">
-        <v>0.411387203070234</v>
+        <v>0.891634984267803</v>
       </c>
       <c r="D21" t="n">
-        <v>0.661732421804452</v>
+        <v>0.737215563806988</v>
       </c>
       <c r="E21" t="n">
-        <v>0.74700931160373</v>
+        <v>2.39500190379072</v>
       </c>
       <c r="F21" t="n">
-        <v>2.04921397688923</v>
+        <v>4.13218663561427</v>
       </c>
       <c r="G21" t="s">
         <v>57</v>
@@ -3836,19 +3836,19 @@
         <v>67</v>
       </c>
       <c r="B22" t="n">
-        <v>1.9059503620883</v>
+        <v>1.4274718624925</v>
       </c>
       <c r="C22" t="n">
-        <v>1.15590032650474</v>
+        <v>0.503838447130369</v>
       </c>
       <c r="D22" t="n">
-        <v>1.19746808526891</v>
+        <v>0.716343499210468</v>
       </c>
       <c r="E22" t="n">
-        <v>4.14450605273849</v>
+        <v>1.15271445462066</v>
       </c>
       <c r="F22" t="n">
-        <v>2.37707039900009</v>
+        <v>1.45602214268836</v>
       </c>
       <c r="G22" t="s">
         <v>58</v>
@@ -3859,19 +3859,19 @@
         <v>68</v>
       </c>
       <c r="B23" t="n">
-        <v>1.42251699055475</v>
+        <v>1.24900141447276</v>
       </c>
       <c r="C23" t="n">
-        <v>1.07293041085584</v>
+        <v>0.427428638090227</v>
       </c>
       <c r="D23" t="n">
-        <v>1.1862966652738</v>
+        <v>0.684209736113797</v>
       </c>
       <c r="E23" t="n">
-        <v>3.82166462142928</v>
+        <v>0.991241582492815</v>
       </c>
       <c r="F23" t="n">
-        <v>2.05671887868381</v>
+        <v>1.25186859178974</v>
       </c>
       <c r="G23" t="s">
         <v>58</v>

</xml_diff>